<commit_message>
new analyses, figures, etc.
</commit_message>
<xml_diff>
--- a/Data/Thesis/Tidy/BrownTrout_OccuMod_Table_v2.xlsx
+++ b/Data/Thesis/Tidy/BrownTrout_OccuMod_Table_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="432">
   <si>
     <t>p</t>
   </si>
@@ -1322,6 +1322,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1639,7 +1642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1754,6 +1757,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1799,9 +1811,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2126,7 +2155,7 @@
   <dimension ref="A1:H283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9496,197 +9525,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>361.84755906976699</v>
+      </c>
+      <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="E2" s="3">
+        <v>9.7586650394221E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>344.73128000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" s="3">
+        <v>361.86975846153803</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.21993917710392E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>9.6509457568196705E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>347.00821999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>361.96630906976702</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.118749999999977</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9.1961104025167606E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>344.85003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>362.43089906976701</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.583339999999964</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7.28986926451132E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>345.31461999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>361.84755906976699</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>9.7586650394221E-2</v>
-      </c>
-      <c r="H2">
-        <v>344.73128000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>361.86975846153803</v>
-      </c>
-      <c r="F3">
-        <v>2.21993917710392E-2</v>
-      </c>
-      <c r="G3">
-        <v>9.6509457568196705E-2</v>
-      </c>
-      <c r="H3">
-        <v>347.00821999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>361.96630906976702</v>
-      </c>
-      <c r="F4">
-        <v>0.118749999999977</v>
-      </c>
-      <c r="G4">
-        <v>9.1961104025167606E-2</v>
-      </c>
-      <c r="H4">
-        <v>344.85003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>362.43089906976701</v>
-      </c>
-      <c r="F5">
-        <v>0.583339999999964</v>
-      </c>
-      <c r="G5">
-        <v>7.28986926451132E-2</v>
-      </c>
-      <c r="H5">
-        <v>345.31461999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="3">
+        <v>362.50722999999999</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.65967093023255097</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7.0168903317133199E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>343.10097999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>362.50722999999999</v>
-      </c>
-      <c r="F6">
-        <v>0.65967093023255097</v>
-      </c>
-      <c r="G6">
-        <v>7.0168903317133199E-2</v>
-      </c>
-      <c r="H6">
-        <v>343.10097999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="8">
         <v>362.88816000000003</v>
       </c>
-      <c r="F7">
+      <c r="D7" s="8">
         <v>1.04060093023259</v>
       </c>
-      <c r="G7">
+      <c r="E7" s="8">
         <v>5.7999839320127498E-2</v>
       </c>
-      <c r="H7">
+      <c r="F7" s="8">
         <v>343.48191000000003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>